<commit_message>
Update Group Member apis and BE doc
</commit_message>
<xml_diff>
--- a/AppNote.xlsx
+++ b/AppNote.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Group" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">API!$A$1:$E$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">API!$A$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="125">
   <si>
     <t>Completion status</t>
   </si>
@@ -321,9 +321,6 @@
     <t>Post: Meetings/Instant</t>
   </si>
   <si>
-    <t>Update Invite Student</t>
-  </si>
-  <si>
     <t>PUT: Meetings/Schedule/id/Start</t>
   </si>
   <si>
@@ -336,9 +333,6 @@
     <t>GroupMember/Request/Group/groupId</t>
   </si>
   <si>
-    <t>GroupMember/Invite/Group/groupId</t>
-  </si>
-  <si>
     <t>Get join invite for group</t>
   </si>
   <si>
@@ -346,6 +340,60 @@
   </si>
   <si>
     <t>GET: Subjects</t>
+  </si>
+  <si>
+    <t>Post: aGroupMember/Invite</t>
+  </si>
+  <si>
+    <t>Get: GroupMember/Invite/Group/groupId</t>
+  </si>
+  <si>
+    <t>Update Invite Student message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accept join request for group </t>
+  </si>
+  <si>
+    <t>Get join invite for student</t>
+  </si>
+  <si>
+    <t>Request join group for Student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accept join invite for student </t>
+  </si>
+  <si>
+    <t>Decline join invite for student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decline join request for group </t>
+  </si>
+  <si>
+    <t>Get join request for student</t>
+  </si>
+  <si>
+    <t>Update group join request message</t>
+  </si>
+  <si>
+    <t>Post: GroupMembers/Request</t>
+  </si>
+  <si>
+    <t>PUT: GroupMember/Request/{inviteId}/Accept</t>
+  </si>
+  <si>
+    <t>PUT: GroupMember/Request/{inviteId}/Decline</t>
+  </si>
+  <si>
+    <t>PUT: GroupMember/Invite/{inviteId}/Accept</t>
+  </si>
+  <si>
+    <t>PUT: GroupMember/Invite/{inviteId}/Decline</t>
+  </si>
+  <si>
+    <t>GET: GroupMember/Invite/Student/{studentId}</t>
+  </si>
+  <si>
+    <t>GET: GroupMember/Request/Student/{studentId}</t>
   </si>
 </sst>
 </file>
@@ -895,16 +943,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.42578125" bestFit="1" customWidth="1"/>
@@ -1112,12 +1160,14 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1183,16 +1233,16 @@
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="A19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1200,263 +1250,327 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="A20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="A21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="C37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="b">
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1473,8 +1587,64 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E31"/>
+  <autoFilter ref="A1:E38"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add search group api
</commit_message>
<xml_diff>
--- a/AppNote.xlsx
+++ b/AppNote.xlsx
@@ -114,9 +114,6 @@
     <t>Delete/Cancle schedule meeting</t>
   </si>
   <si>
-    <t>Search Student</t>
-  </si>
-  <si>
     <t>Invite Student</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>POST: Groups/</t>
   </si>
   <si>
-    <t>Chưa cập nhật</t>
-  </si>
-  <si>
     <t>Get live meeting for group</t>
   </si>
   <si>
@@ -394,6 +388,12 @@
   </si>
   <si>
     <t>GET: GroupMember/Request/Student/{studentId}</t>
+  </si>
+  <si>
+    <t>Search Student for new member</t>
+  </si>
+  <si>
+    <t>thêm groupId để ko tìm thấy những student đã thêm vào group</t>
   </si>
 </sst>
 </file>
@@ -946,7 +946,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +955,7 @@
     <col min="2" max="2" width="50.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -980,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -995,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1010,7 +1010,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
@@ -1025,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1040,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -1055,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -1085,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -1115,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>11</v>
@@ -1130,10 +1130,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>12</v>
@@ -1160,10 +1160,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>23</v>
@@ -1175,16 +1175,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>13</v>
@@ -1207,10 +1207,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>27</v>
@@ -1222,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
@@ -1237,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>15</v>
@@ -1246,7 +1246,7 @@
         <v>23</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1254,10 +1254,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>27</v>
@@ -1269,10 +1269,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>27</v>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>27</v>
@@ -1297,7 +1297,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
@@ -1306,7 +1306,7 @@
         <v>27</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1314,10 +1314,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>27</v>
@@ -1329,10 +1329,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>27</v>
@@ -1344,10 +1344,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>22</v>
@@ -1359,10 +1359,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>22</v>
@@ -1374,10 +1374,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>22</v>
@@ -1389,10 +1389,10 @@
         <v>1</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>22</v>
@@ -1404,10 +1404,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>22</v>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>22</v>
@@ -1432,10 +1432,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>23</v>
@@ -1447,10 +1447,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>23</v>
@@ -1462,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>27</v>
@@ -1477,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>24</v>
@@ -1494,10 +1494,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>27</v>
@@ -1509,7 +1509,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>30</v>
@@ -1524,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>26</v>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>27</v>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>27</v>
@@ -1665,7 +1665,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1708,7 +1708,7 @@
     <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -1743,10 +1743,10 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
@@ -1758,10 +1758,10 @@
     </row>
     <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1813,54 +1813,54 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q14" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
@@ -1872,68 +1872,68 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1953,27 +1953,27 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2011,7 +2011,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -2054,7 +2054,7 @@
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -2125,7 +2125,7 @@
     <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add signal R doc
</commit_message>
<xml_diff>
--- a/AppNote.xlsx
+++ b/AppNote.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
-    <sheet name="Meeting" sheetId="2" r:id="rId2"/>
-    <sheet name="Group" sheetId="3" r:id="rId3"/>
+    <sheet name="Meeting Hub" sheetId="4" r:id="rId2"/>
+    <sheet name="Meeting" sheetId="2" r:id="rId3"/>
+    <sheet name="Group" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">API!$A$1:$E$41</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="134">
   <si>
     <t>Completion status</t>
   </si>
@@ -397,13 +398,165 @@
   </si>
   <si>
     <t>Search group for student to join new group</t>
+  </si>
+  <si>
+    <t>FE Connect</t>
+  </si>
+  <si>
+    <t>FE Catch từ be</t>
+  </si>
+  <si>
+    <t>this.chatHubConnection = new HubConnectionBuilder()
+  .withUrl(this.hubUrl + 'meetinghub?meetingId=' + meetingId, {
+    accessTokenFactory: () =&gt; user.token})
+  .withAutomaticReconnect().build();
+this.chatHubConnection.start().catch(err =&gt; console.log(err));</t>
+  </si>
+  <si>
+    <t>Thông báo có thành viên mới trong Meeting "UserOnlineInMeeting"</t>
+  </si>
+  <si>
+    <t>BE gửi</t>
+  </si>
+  <si>
+    <r>
+      <t>SendAsync(“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>UserOnlineInMeeting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">”, MemberSignalrDto </t>
+    </r>
+  </si>
+  <si>
+    <t>FE bắt</t>
+  </si>
+  <si>
+    <r>
+      <t>this</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.chatHubConnection.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>on</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'UserOnlineInMeeting'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFB8D7A3"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Member</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {
+  //code xử lí fe, chắc là đẩy username vô cái meet
+  this.oneOnlineUserSource.next(user);
+  this.toastr.success(user.displayName + ' has join room!')</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +570,71 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2E74B5"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF008000"/>
+      <name val="Cascadia Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FFA31515"/>
+      <name val="Cascadia Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFDCDCAA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFB8D7A3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -444,7 +662,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -593,12 +811,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -640,6 +884,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -948,7 +1208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
@@ -1666,6 +1926,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X28"/>
   <sheetViews>
@@ -2011,7 +2330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R22"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add validator for Update account
</commit_message>
<xml_diff>
--- a/AppNote.xlsx
+++ b/AppNote.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="133">
   <si>
     <t>Completion status</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>Chỉ có leader có đặt lại lịch 1 schedule meeting</t>
-  </si>
-  <si>
-    <t>ScheduleStart phải trễ hơn bây giờ, và ScheduleEnd phải cùng ngày ScheduleStart</t>
   </si>
   <si>
     <t>Group</t>
@@ -852,6 +849,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -884,22 +897,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1378,10 +1375,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>20</v>
@@ -1393,7 +1390,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>40</v>
@@ -1408,10 +1405,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>20</v>
@@ -1423,10 +1420,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>21</v>
@@ -1439,7 +1436,7 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>20</v>
@@ -1451,16 +1448,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1468,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
@@ -1483,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>39</v>
@@ -1498,7 +1495,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>12</v>
@@ -1513,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>13</v>
@@ -1522,7 +1519,7 @@
         <v>21</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,10 +1527,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>25</v>
@@ -1545,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>29</v>
@@ -1561,7 +1558,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
@@ -1573,7 +1570,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>15</v>
@@ -1582,7 +1579,7 @@
         <v>25</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1590,10 +1587,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>25</v>
@@ -1605,10 +1602,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>25</v>
@@ -1620,10 +1617,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>20</v>
@@ -1635,10 +1632,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>20</v>
@@ -1650,10 +1647,10 @@
         <v>1</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>20</v>
@@ -1665,10 +1662,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>20</v>
@@ -1680,10 +1677,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>20</v>
@@ -1696,7 +1693,7 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>20</v>
@@ -1708,10 +1705,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>21</v>
@@ -1723,10 +1720,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>21</v>
@@ -1738,10 +1735,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>25</v>
@@ -1753,7 +1750,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>22</v>
@@ -1770,10 +1767,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>25</v>
@@ -1785,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>28</v>
@@ -1800,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>24</v>
@@ -1816,7 +1813,7 @@
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>25</v>
@@ -1829,7 +1826,7 @@
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>25</v>
@@ -1929,7 +1926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1939,43 +1936,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>126</v>
+      <c r="A1" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>128</v>
+      <c r="A2" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+    <row r="8" spans="1:1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="57" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1988,8 +1985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:I7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,136 +1996,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="16"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="15"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="15"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="B5" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="B6" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="15"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="21"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2154,7 +2151,7 @@
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -2162,15 +2159,15 @@
         <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -2181,7 +2178,7 @@
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -2189,21 +2186,21 @@
         <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q14" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="Q14" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2213,7 +2210,7 @@
         <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -2221,15 +2218,15 @@
         <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -2237,10 +2234,10 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2251,7 +2248,7 @@
         <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2259,32 +2256,32 @@
         <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="15"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="21"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2299,11 +2296,6 @@
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2345,142 +2337,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10"/>
+      <c r="A1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="16"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="15"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="15"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="15"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="21"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="15"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="21"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>